<commit_message>
update documentation of matrix equilibration log
</commit_message>
<xml_diff>
--- a/matrix_equilibration/matrix_equilibration_log_30p30n.xlsx
+++ b/matrix_equilibration/matrix_equilibration_log_30p30n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-37400" yWindow="-5540" windowWidth="19860" windowHeight="22180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-32860" yWindow="460" windowWidth="19860" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="67">
   <si>
     <t>tolerance =</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>eval order</t>
+  </si>
+  <si>
+    <t>CC=g++-6    CFLAGS=-std=c++11 -g -Wall -O2 -fno-unsafe-math-optimizations -fopenmp</t>
   </si>
 </sst>
 </file>
@@ -2599,10 +2602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H59"/>
+  <dimension ref="A3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2613,9 +2616,14 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>